<commit_message>
add kpi analysis function
</commit_message>
<xml_diff>
--- a/config/OuterData.xlsx
+++ b/config/OuterData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15480" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="15480" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="TOTAL&lt;ALL&gt;" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,17 @@
     <sheet name="FTPIE&lt;UE&gt;" sheetId="3" r:id="rId3"/>
     <sheet name="COVIE&lt;UE&gt;" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="114210" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>&lt;NAME&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -163,72 +168,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;FTP_RSRP_Max&gt;</t>
-  </si>
-  <si>
-    <t>&lt;FTP_RSRP_Min&gt;</t>
-  </si>
-  <si>
     <t>&lt;FTP_RSRP_Avg&gt;</t>
   </si>
   <si>
     <t>&lt;FTP_RSRP_Cnt&gt;</t>
   </si>
   <si>
-    <t>&lt;FTP_RSRQ_Max&gt;</t>
-  </si>
-  <si>
-    <t>&lt;FTP_RSRQ_Min&gt;</t>
-  </si>
-  <si>
     <t>&lt;FTP_RSRQ_Avg&gt;</t>
   </si>
   <si>
     <t>&lt;FTP_RSRQ_Cnt&gt;</t>
   </si>
   <si>
-    <t>&lt;FTP_RSSI_Max&gt;</t>
-  </si>
-  <si>
-    <t>&lt;FTP_RSSI_Min&gt;</t>
-  </si>
-  <si>
     <t>&lt;FTP_RSSI_Avg&gt;</t>
   </si>
   <si>
     <t>&lt;FTP_RSSI_Cnt&gt;</t>
   </si>
   <si>
-    <t>&lt;FTP_SINR_Max&gt;</t>
-  </si>
-  <si>
-    <t>&lt;FTP_SINR_Min&gt;</t>
-  </si>
-  <si>
     <t>&lt;FTP_SINR_Avg&gt;</t>
   </si>
   <si>
     <t>&lt;FTP_SINR_Cnt&gt;</t>
   </si>
   <si>
-    <t>&lt;FTP_DL_BLER_Max&gt;</t>
-  </si>
-  <si>
-    <t>&lt;FTP_DL_BLER_Min&gt;</t>
-  </si>
-  <si>
     <t>&lt;FTP_DL_BLER_Avg&gt;</t>
   </si>
   <si>
     <t>&lt;FTP_DL_BLER_Cnt&gt;</t>
   </si>
   <si>
-    <t>&lt;FTP_TxPwr_Max&gt;</t>
-  </si>
-  <si>
-    <t>&lt;FTP_TxPwr_Min&gt;</t>
-  </si>
-  <si>
     <t>&lt;FTP_TxPwr_Avg&gt;</t>
   </si>
   <si>
@@ -241,24 +210,12 @@
     <t>&lt;FTP_DL_Time_Cnt&gt;</t>
   </si>
   <si>
-    <t>&lt;FTP_DL_Size_Max&gt;</t>
-  </si>
-  <si>
-    <t>&lt;FTP_DL_Size_Min&gt;</t>
-  </si>
-  <si>
     <t>&lt;FTP_DL_Size_Avg&gt;</t>
   </si>
   <si>
     <t>&lt;FTP_DL_Size_Cnt&gt;</t>
   </si>
   <si>
-    <t>&lt;FTP_DL_Rate_Max&gt;</t>
-  </si>
-  <si>
-    <t>&lt;FTP_DL_Rate_Min&gt;</t>
-  </si>
-  <si>
     <t>&lt;FTP_DL_Rate_Avg&gt;</t>
   </si>
   <si>
@@ -347,34 +304,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;SINR_Avg_1&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SINR_Avg_2</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_2&gt;</t>
-  </si>
-  <si>
     <t>SINR_Avg_3</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_3&gt;</t>
-  </si>
-  <si>
     <t>SINR_Avg_4</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_4&gt;</t>
-  </si>
-  <si>
     <t>SINR_Avg_5</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_5&gt;</t>
-  </si>
-  <si>
     <t>SINR_Avg_S_Count</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -382,61 +323,78 @@
     <t>SINR_Avg_1_S_Count</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_1_S_Count&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SINR_Avg_2_S_Count</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_2_S_Count&gt;</t>
-  </si>
-  <si>
     <t>SINR_Avg_3_S_Count</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_3_S_Count&gt;</t>
-  </si>
-  <si>
     <t>SINR_Avg_4_S_Count</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_4_S_Count&gt;</t>
-  </si>
-  <si>
     <t>SINR_Avg_5_S_Count</t>
   </si>
   <si>
-    <t>&lt;SINR_Avg_5_S_Count&gt;</t>
-  </si>
-  <si>
-    <t>&lt;SINR_Avg_S_Count&gt;</t>
+    <t>[-110,-100)</t>
+  </si>
+  <si>
+    <t>[-100,-90)</t>
+  </si>
+  <si>
+    <t>[-141,-110)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-22,0)</t>
+  </si>
+  <si>
+    <t>[0,5)</t>
+  </si>
+  <si>
+    <t>[5,15)</t>
+  </si>
+  <si>
+    <t>[15,22)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-90,-85)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUCCH_Power</t>
+  </si>
+  <si>
+    <t>SINR1</t>
+  </si>
+  <si>
+    <t>RSRP_minus</t>
+  </si>
+  <si>
+    <t>&lt;RSRP_minus&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -450,7 +408,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor indexed="22"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,27 +422,145 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -493,7 +569,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -501,22 +577,22 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,136 +601,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,58 +626,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,11 +754,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1083,27 +1046,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="17.25" customWidth="1"/>
-    <col min="3" max="3" width="9.125" customWidth="1"/>
-    <col min="4" max="5" width="17.25" customWidth="1"/>
+    <col min="1" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="29.375" customWidth="1"/>
+    <col min="4" max="5" width="17.125" customWidth="1"/>
     <col min="6" max="6" width="10.375" customWidth="1"/>
-    <col min="7" max="8" width="17.25" customWidth="1"/>
-    <col min="9" max="9" width="10.25" customWidth="1"/>
-    <col min="10" max="11" width="17.25" customWidth="1"/>
+    <col min="7" max="8" width="17.125" customWidth="1"/>
+    <col min="9" max="9" width="10.125" customWidth="1"/>
+    <col min="10" max="11" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1116,7 +1079,7 @@
       <c r="J1" s="14"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25" thickBot="1">
+    <row r="2" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -1129,302 +1092,292 @@
       <c r="J2" s="17"/>
       <c r="K2" s="18"/>
     </row>
-    <row r="4" spans="1:11" ht="14.25" thickBot="1"/>
-    <row r="5" spans="1:11" ht="15">
+    <row r="4" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
+      <c r="B5" s="1">
+        <v>-77</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="H5" s="1"/>
       <c r="J5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15">
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>37</v>
+      <c r="B6" s="2">
+        <v>-97</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="H6" s="2"/>
       <c r="J6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>38</v>
+      <c r="B7" s="2">
+        <v>-88.039033457249076</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="J7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>39</v>
+      <c r="B8" s="3">
+        <v>1614</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="G8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="H8" s="3"/>
       <c r="J8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="14.25" thickBot="1"/>
-    <row r="12" spans="1:11" ht="30">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="D12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="G12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="J12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="D13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="E13" s="2"/>
       <c r="G13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="J13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="D14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="G14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="J14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="D15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="E15" s="3"/>
       <c r="G15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="H15" s="3"/>
       <c r="J15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A19" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A20" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A21" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A22" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A23" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
         <v>95</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B34">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15">
-      <c r="A19" s="12" t="s">
+      <c r="B35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
         <v>97</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B40">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15">
-      <c r="A20" s="12" t="s">
+      <c r="B42">
+        <v>2918</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
         <v>99</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15">
-      <c r="A21" s="12" t="s">
+      <c r="B44" t="s">
         <v>101</v>
-      </c>
-      <c r="B21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15">
-      <c r="A22" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15">
-      <c r="A23" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1433,119 +1386,129 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="38.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="45.75" thickBot="1">
+    <row r="1" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>20</v>
@@ -1578,61 +1541,66 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="7" customFormat="1">
+    <row r="2" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" thickBot="1">
+    <row r="1" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>4</v>
@@ -1659,37 +1627,42 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix FileReader can not process the file_group bug
</commit_message>
<xml_diff>
--- a/config/OuterData.xlsx
+++ b/config/OuterData.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="TOTAL&lt;ALL&gt;" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="114210" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
   <si>
     <t>RSRP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,6 +170,66 @@
   </si>
   <si>
     <t>&lt;FTP_DL[4]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#RSRP[0]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#RSRP[1]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#RSRP[2]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#RSRP[3]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#RSRP[4]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#SINR[0]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#SINR[1]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#SINR[2]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#SINR[3]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#SINR[4]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#FTP_DL[0]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#FTP_DL[1]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#FTP_DL[2]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#FTP_DL[3]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;ningbo#FTP_DL[4]&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -247,8 +307,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -311,7 +377,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -320,6 +386,7 @@
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -328,6 +395,7 @@
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -620,15 +688,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
@@ -847,6 +917,222 @@
       </c>
       <c r="F14" t="e">
         <f>F13/G13*100</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="e">
+        <f>B18+C18+D18+E18+F18</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="e">
+        <f>B18/G18*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C19" t="e">
+        <f>C18/G18*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" t="e">
+        <f>D18/G18*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" t="e">
+        <f>E18/G18*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" t="e">
+        <f>F18/G18*100</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="e">
+        <f>B24+C24+D24+E24+F24</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="e">
+        <f>B24/G24*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C25" t="e">
+        <f>C24/G24*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D25" t="e">
+        <f>D24/G24*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E25" t="e">
+        <f>E24/G24*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F25" t="e">
+        <f>F24/G24*100</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" t="e">
+        <f>B29+C29+D29+E29+F29</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="e">
+        <f>B29/G29*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C30" t="e">
+        <f>C29/G29*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D30" t="e">
+        <f>D29/G29*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E30" t="e">
+        <f>E29/G29*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F30" t="e">
+        <f>F29/G29*100</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>